<commit_message>
java.net.SocketException: Software caused connection abort: socket write error困惑了一天还是没解决
</commit_message>
<xml_diff>
--- a/api/ExcelForData/testData.xlsx
+++ b/api/ExcelForData/testData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\eclipse-workspace\api_automation\api\ExcelForData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23895" windowHeight="10350" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="6" r:id="rId1"/>
@@ -15,13 +20,15 @@
     <sheet name="quickbuy" sheetId="7" r:id="rId6"/>
     <sheet name="address" sheetId="5" r:id="rId7"/>
     <sheet name="test" sheetId="8" r:id="rId8"/>
+    <sheet name="testgift" sheetId="9" r:id="rId9"/>
+    <sheet name="buy" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="205">
   <si>
     <t>测试服务器</t>
   </si>
@@ -818,20 +825,43 @@
     <t>jsonParam</t>
   </si>
   <si>
-    <t>{"contact":"张大爷","phone":13714672776,"gender":0,"regionId":813395,"latitude":22.408965,"longitude":113.826119,"room1":"1111","village":"东角山","city1":"深圳","addressNaviId":18039,"building":"自动化测试楼栋C栋（勿删）","addressBuildingId":256}</t>
+    <t>成功</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"dealId":994140,"selected":true,"dealCount":1}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"dealId":991824,"odLabelId":"-1","limitFlag":false,"selected":false,"specId":924116,"dealCount":1}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jsonParam(将自动化商品1添加到购物车)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许购买</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"contact":"99","phone":13714672776,"gender":1,"regionId":813395,"latitude":22.408965,"longitude":113.826119,"room1":"9999","village":"东角山","city1":"深圳","addressNaviId":18039,"building":"自动化测试楼栋C栋（勿删）","addressBuildingId":256}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>expectValue</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,148 +888,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,7 +906,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399914548173467"/>
+        <fgColor theme="4" tint="0.39988402966399123"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,198 +918,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399945066682943"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1219,251 +931,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1496,61 +966,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1808,35 +1234,75 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="100.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="12" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
@@ -1846,7 +1312,7 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1898,32 +1364,31 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://release.thy360.com" tooltip="http://release.thy360.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="http://172.16.0.21"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="http://release.thy360.com"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.625" style="8" customWidth="1"/>
     <col min="2" max="2" width="81.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1931,7 +1396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1939,7 +1404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -1947,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -1955,7 +1420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -1963,7 +1428,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -1971,7 +1436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
@@ -1979,7 +1444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1987,7 +1452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>28</v>
       </c>
@@ -1995,7 +1460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
@@ -2003,7 +1468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
@@ -2011,7 +1476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
@@ -2020,28 +1485,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="64.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -2052,7 +1516,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -2063,7 +1527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -2074,7 +1538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -2085,7 +1549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -2096,7 +1560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -2107,7 +1571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -2118,7 +1582,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -2129,7 +1593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -2140,7 +1604,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2151,7 +1615,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2162,7 +1626,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -2173,7 +1637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -2184,7 +1648,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
@@ -2195,7 +1659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -2206,7 +1670,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -2217,7 +1681,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -2228,7 +1692,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -2239,7 +1703,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -2250,7 +1714,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -2261,7 +1725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -2272,7 +1736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
@@ -2283,7 +1747,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -2294,7 +1758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
@@ -2305,7 +1769,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>86</v>
       </c>
@@ -2316,7 +1780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
@@ -2327,7 +1791,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
@@ -2338,7 +1802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
@@ -2349,7 +1813,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
@@ -2360,7 +1824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>96</v>
       </c>
@@ -2371,7 +1835,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>98</v>
       </c>
@@ -2382,7 +1846,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>100</v>
       </c>
@@ -2393,7 +1857,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>102</v>
       </c>
@@ -2404,7 +1868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>104</v>
       </c>
@@ -2415,7 +1879,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
@@ -2426,7 +1890,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
@@ -2437,7 +1901,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -2448,7 +1912,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>112</v>
       </c>
@@ -2459,7 +1923,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
@@ -2470,7 +1934,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>116</v>
       </c>
@@ -2481,7 +1945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>118</v>
       </c>
@@ -2492,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>120</v>
       </c>
@@ -2503,7 +1967,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>122</v>
       </c>
@@ -2514,7 +1978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -2526,21 +1990,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
@@ -2552,7 +2015,7 @@
     <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>126</v>
       </c>
@@ -2566,7 +2029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>130</v>
       </c>
@@ -2580,7 +2043,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>134</v>
       </c>
@@ -2594,7 +2057,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>137</v>
       </c>
@@ -2608,7 +2071,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>139</v>
       </c>
@@ -2622,7 +2085,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>130</v>
       </c>
@@ -2637,21 +2100,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="108.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
@@ -2662,7 +2124,7 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>141</v>
       </c>
@@ -2670,7 +2132,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>142</v>
       </c>
@@ -2679,21 +2141,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
@@ -2711,7 +2172,7 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -2752,7 +2213,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>157</v>
       </c>
@@ -2793,7 +2254,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -2832,7 +2293,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>157</v>
       </c>
@@ -2873,7 +2334,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>157</v>
       </c>
@@ -2914,7 +2375,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>157</v>
       </c>
@@ -2955,7 +2416,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>157</v>
       </c>
@@ -2996,7 +2457,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>157</v>
       </c>
@@ -3037,7 +2498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>157</v>
       </c>
@@ -3078,7 +2539,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>157</v>
       </c>
@@ -3117,7 +2578,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>157</v>
       </c>
@@ -3158,7 +2619,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>157</v>
       </c>
@@ -3199,7 +2660,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>157</v>
       </c>
@@ -3240,7 +2701,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>157</v>
       </c>
@@ -3281,7 +2742,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>157</v>
       </c>
@@ -3322,7 +2783,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>157</v>
       </c>
@@ -3363,7 +2824,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
@@ -3404,7 +2865,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>157</v>
       </c>
@@ -3445,7 +2906,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>157</v>
       </c>
@@ -3484,7 +2945,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
@@ -3523,7 +2984,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>157</v>
       </c>
@@ -3564,7 +3025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>157</v>
       </c>
@@ -3605,7 +3066,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>157</v>
       </c>
@@ -3646,7 +3107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>157</v>
       </c>
@@ -3687,7 +3148,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>157</v>
       </c>
@@ -3728,7 +3189,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>157</v>
       </c>
@@ -3767,7 +3228,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>157</v>
       </c>
@@ -3808,7 +3269,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>157</v>
       </c>
@@ -3849,7 +3310,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>157</v>
       </c>
@@ -3890,7 +3351,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>157</v>
       </c>
@@ -3932,26 +3393,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I14" r:id="rId1" display="137$46&amp;27@6"/>
+    <hyperlink ref="I14" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="182.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="215.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1"/>
     <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
@@ -3960,24 +3420,65 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="48.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="12" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="37" customHeight="1" spans="1:2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>